<commit_message>
updated codebooks cohort and flares
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_cohort_{ImmDis}.xlsx
+++ b/i_codebooks/D3_cohort_{ImmDis}.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Parameters" sheetId="5" r:id="rId3"/>
     <sheet name="Example" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
   <si>
     <t>metadata_content</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>date when the person is first found with {ImmDis}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whether the person enters follow up </t>
   </si>
   <si>
     <t>yes</t>
@@ -195,15 +192,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>entering_follow_up_{ImmDis}_COMP_{comp{ImmDis}}</t>
-  </si>
-  <si>
-    <t>cohort_entry_date_{ImmDis}_COMP_{comp{ImmDis}}</t>
-  </si>
-  <si>
-    <t>start_follow_up_{ImmDis}_COMP_{comp{ImmDis}}</t>
-  </si>
-  <si>
     <t>ImmDis</t>
   </si>
   <si>
@@ -240,40 +228,7 @@
     <t>study_exit_date</t>
   </si>
   <si>
-    <t>comp[["E_GRAVES_AESI"]]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][1]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][2]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][3]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][4]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][5]</t>
-  </si>
-  <si>
-    <t>comp[["E_GRAVES_AESI"]][6]</t>
-  </si>
-  <si>
     <t>…</t>
-  </si>
-  <si>
-    <t>comp[["D_HEPATITISAUTOIMMUNE_AESI"]][1]</t>
-  </si>
-  <si>
-    <t>comp[["D_HEPATITISAUTOIMMUNE_AESI"]]</t>
-  </si>
-  <si>
-    <t>comp[["D_HEPATITISAUTOIMMUNE_AESI"]][2]</t>
-  </si>
-  <si>
-    <t>ImmDis comp{ImmDis}</t>
   </si>
   <si>
     <t>entering_follow_up_postponed_{ImmDis}</t>
@@ -292,6 +247,123 @@
 otehwrsie if entering_follow_up_{ImmDis} == 1 &amp; entering_follow_up_postponed_{ImmDis} == 1:
 date of last vasscine in window of 90 days + 90
 otherwise: null</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>cohort_entry_date_{ImmDis}_{group_of_prompt}</t>
+  </si>
+  <si>
+    <t>group_of_prompt</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>groups_of_prompts</t>
+  </si>
+  <si>
+    <t>HOSP_DISP</t>
+  </si>
+  <si>
+    <t>07_algorithms</t>
+  </si>
+  <si>
+    <t>whether the person enters follow up of {ImmDis} when the prompts are restricted to {group_of_prompt}</t>
+  </si>
+  <si>
+    <t>entering_follow_up_{ImmDis}_{group_of_prompt}</t>
+  </si>
+  <si>
+    <t>start_follow_up_{ImmDis}_{group_of_prompt}</t>
+  </si>
+  <si>
+    <t>date when the person enters the follow up for {ImmDis}</t>
+  </si>
+  <si>
+    <t>whether the person enters follow up for {ImmDis}</t>
+  </si>
+  <si>
+    <t>date when the person enters the follow up for {ImmDis}  when the prompts are restricted to {group_of_prompt}</t>
+  </si>
+  <si>
+    <t>date when the person is first found for {ImmDis} when the prompts are restricted to {group_of_prompt}</t>
+  </si>
+  <si>
+    <t>reason why the persons does not enter follow up (if any)  when the prompts are restricted to {group_of_prompt}</t>
+  </si>
+  <si>
+    <t>if the person is vaccinated during the first 9'0 days after cohort_entry_date, then  their entry is potsponed to 90 days after the vaccination (if vaccinated more than once in a 90-days window, the computation of 90 days is restarted)</t>
+  </si>
+  <si>
+    <t>ImmDis group_of_prompt</t>
+  </si>
+  <si>
+    <t>cohort_entry_date_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>cause_for_not_entering_followup_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>entering_follow_up_postponed_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>entering_follow_up_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>start_follow_up_E_GRAVES_AESI</t>
+  </si>
+  <si>
+    <t>cohort_entry_date_E_GRAVES_AESI_PC</t>
+  </si>
+  <si>
+    <t>entering_follow_up_E_GRAVES_AESI_PC</t>
+  </si>
+  <si>
+    <t>start_follow_up_E_GRAVES_AESI_PC</t>
+  </si>
+  <si>
+    <t>cohort_entry_date_E_GRAVES_AESI_HOSP_DISP</t>
+  </si>
+  <si>
+    <t>cause_for_not_entering_followup_E_GRAVES_AESI_HOSP_DISP</t>
+  </si>
+  <si>
+    <t>entering_follow_up_postponed_E_GRAVES_AESI_HOSP_DISP</t>
+  </si>
+  <si>
+    <t>entering_follow_up_E_GRAVES_AESI_HOSP_DISP</t>
+  </si>
+  <si>
+    <t>start_follow_up_E_GRAVES_AESI_HOSP_DISP</t>
+  </si>
+  <si>
+    <t>cohort_entry_date_E_GRAVES_AESI_HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>entering_follow_up_E_GRAVES_AESI_HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>start_follow_up_E_GRAVES_AESI_HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>cause_for_not_entering_followup_E_GRAVES_AESI_PC</t>
+  </si>
+  <si>
+    <t>entering_follow_up_postponed_E_GRAVES_AESI_PC</t>
+  </si>
+  <si>
+    <t>cause_for_not_entering_followup_E_GRAVES_AESI_HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>entering_follow_up_postponed_E_GRAVES_AESI_HOSP_SPEC_DISP</t>
+  </si>
+  <si>
+    <t>for some data sources, some groups may be not caculated; for TEST only PC and HOSP_DISP are calculates</t>
   </si>
 </sst>
 </file>
@@ -370,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -397,6 +469,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -680,7 +758,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -777,13 +855,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:A11"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +921,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -854,61 +932,61 @@
         <v>48</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="I5" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -916,57 +994,103 @@
         <v>46</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
+      <c r="B8" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="F8" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K8" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="F9" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>80</v>
+      <c r="B13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -979,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,6 +1113,7 @@
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.44140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1007,16 +1132,16 @@
       <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1027,10 +1152,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -1041,10 +1166,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -1055,10 +1180,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -1069,10 +1194,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -1083,10 +1208,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
@@ -1097,10 +1222,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -1111,10 +1236,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -1125,10 +1250,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
@@ -1139,10 +1264,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
@@ -1151,108 +1276,80 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
       <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>74</v>
-      </c>
       <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1262,18 +1359,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="8.6640625" style="12"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="12">
+        <v>100</v>
+      </c>
+      <c r="C2" s="12">
+        <v>730</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
+        <v>190</v>
+      </c>
+      <c r="H2" s="12">
+        <v>150</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1</v>
+      </c>
+      <c r="L2" s="12">
+        <v>240</v>
+      </c>
+      <c r="M2" s="12">
+        <v>100</v>
+      </c>
+      <c r="N2" s="12">
+        <v>0</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0</v>
+      </c>
+      <c r="P2" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>190</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>